<commit_message>
add enrichment results output
</commit_message>
<xml_diff>
--- a/results/tables/top_go_under-rep_terms_adj_pvalue_sorted.xlsx
+++ b/results/tables/top_go_under-rep_terms_adj_pvalue_sorted.xlsx
@@ -32,49 +32,49 @@
     <t xml:space="preserve">ontology</t>
   </si>
   <si>
+    <t xml:space="preserve">GO:0003735</t>
+  </si>
+  <si>
+    <t xml:space="preserve">structural constituent of ribosome</t>
+  </si>
+  <si>
+    <t xml:space="preserve">MF</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005198</t>
+  </si>
+  <si>
+    <t xml:space="preserve">structural molecule activity</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0005730</t>
+  </si>
+  <si>
+    <t xml:space="preserve">nucleolus</t>
+  </si>
+  <si>
+    <t xml:space="preserve">CC</t>
+  </si>
+  <si>
+    <t xml:space="preserve">GO:0009987</t>
+  </si>
+  <si>
+    <t xml:space="preserve">cellular process</t>
+  </si>
+  <si>
+    <t xml:space="preserve">BP</t>
+  </si>
+  <si>
     <t xml:space="preserve">GO:0043228</t>
   </si>
   <si>
     <t xml:space="preserve">non-membrane-bounded organelle</t>
   </si>
   <si>
-    <t xml:space="preserve">CC</t>
-  </si>
-  <si>
     <t xml:space="preserve">GO:0043232</t>
   </si>
   <si>
     <t xml:space="preserve">intracellular non-membrane-bounded organelle</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005730</t>
-  </si>
-  <si>
-    <t xml:space="preserve">nucleolus</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0003735</t>
-  </si>
-  <si>
-    <t xml:space="preserve">structural constituent of ribosome</t>
-  </si>
-  <si>
-    <t xml:space="preserve">MF</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0005198</t>
-  </si>
-  <si>
-    <t xml:space="preserve">structural molecule activity</t>
-  </si>
-  <si>
-    <t xml:space="preserve">GO:0009987</t>
-  </si>
-  <si>
-    <t xml:space="preserve">cellular process</t>
-  </si>
-  <si>
-    <t xml:space="preserve">BP</t>
   </si>
 </sst>
 </file>
@@ -404,7 +404,7 @@
   <sheetViews>
     <sheetView workbookViewId="0" zoomScale="100" showGridLines="1" tabSelected="1"/>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15.0" baseColWidth="10"/>
+  <sheetFormatPr defaultRowHeight="15.0"/>
   <sheetData>
     <row r="1">
       <c r="A1" t="s">
@@ -431,13 +431,13 @@
         <v>6</v>
       </c>
       <c r="B2" t="n">
-        <v>66</v>
+        <v>6</v>
       </c>
       <c r="C2" t="n">
-        <v>1305</v>
+        <v>161</v>
       </c>
       <c r="D2" t="n">
-        <v>0</v>
+        <v>0.0498993422015866</v>
       </c>
       <c r="E2" t="s">
         <v>7</v>
@@ -451,13 +451,13 @@
         <v>9</v>
       </c>
       <c r="B3" t="n">
-        <v>66</v>
+        <v>8</v>
       </c>
       <c r="C3" t="n">
-        <v>1305</v>
+        <v>190</v>
       </c>
       <c r="D3" t="n">
-        <v>0</v>
+        <v>0.0498993422015866</v>
       </c>
       <c r="E3" t="s">
         <v>10</v>
@@ -483,67 +483,67 @@
         <v>12</v>
       </c>
       <c r="F4" t="s">
-        <v>8</v>
+        <v>13</v>
       </c>
     </row>
     <row r="5">
       <c r="A5" t="s">
-        <v>13</v>
+        <v>14</v>
       </c>
       <c r="B5" t="n">
-        <v>6</v>
+        <v>179</v>
       </c>
       <c r="C5" t="n">
-        <v>161</v>
+        <v>2338</v>
       </c>
       <c r="D5" t="n">
         <v>0.0498993422015866</v>
       </c>
       <c r="E5" t="s">
-        <v>14</v>
+        <v>15</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
+        <v>16</v>
       </c>
     </row>
     <row r="6">
       <c r="A6" t="s">
-        <v>16</v>
+        <v>17</v>
       </c>
       <c r="B6" t="n">
-        <v>8</v>
+        <v>66</v>
       </c>
       <c r="C6" t="n">
-        <v>190</v>
+        <v>1305</v>
       </c>
       <c r="D6" t="n">
-        <v>0.0498993422015866</v>
+        <v>0</v>
       </c>
       <c r="E6" t="s">
-        <v>17</v>
+        <v>18</v>
       </c>
       <c r="F6" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
     </row>
     <row r="7">
       <c r="A7" t="s">
-        <v>18</v>
+        <v>19</v>
       </c>
       <c r="B7" t="n">
-        <v>179</v>
+        <v>66</v>
       </c>
       <c r="C7" t="n">
-        <v>2338</v>
+        <v>1305</v>
       </c>
       <c r="D7" t="n">
-        <v>0.0498993422015866</v>
+        <v>0</v>
       </c>
       <c r="E7" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="F7" t="s">
-        <v>20</v>
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>